<commit_message>
Modify card counts, and adjust formatting
</commit_message>
<xml_diff>
--- a/SCP_ The Downfall of Site 13 Cards.xlsx
+++ b/SCP_ The Downfall of Site 13 Cards.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achyt\Documents\Site13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achyt\dev\Downfall-Of-Site-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6AF933-A9DC-47BA-8108-4C727D467F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7521683C-32CF-4359-A6EB-C1070C5CD806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1450,9 +1450,9 @@
   </sheetPr>
   <dimension ref="A1:AE876"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A91" sqref="A91"/>
+      <selection pane="topRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3016,7 +3016,8 @@
         <v>125</v>
       </c>
       <c r="D34" s="1">
-        <v>15</v>
+        <f>15-8</f>
+        <v>7</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -3050,7 +3051,7 @@
         <v>125</v>
       </c>
       <c r="D35" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -3084,7 +3085,7 @@
         <v>125</v>
       </c>
       <c r="D36" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -3118,7 +3119,7 @@
         <v>125</v>
       </c>
       <c r="D37" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -3150,7 +3151,7 @@
         <v>137</v>
       </c>
       <c r="D38" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -3182,7 +3183,7 @@
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -3214,7 +3215,7 @@
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -3246,7 +3247,7 @@
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -3276,7 +3277,7 @@
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
@@ -3308,7 +3309,7 @@
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
@@ -3536,7 +3537,7 @@
         <v>171</v>
       </c>
       <c r="D50" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
@@ -4230,7 +4231,7 @@
         <v>231</v>
       </c>
       <c r="D71" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
@@ -4322,7 +4323,7 @@
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
@@ -4354,7 +4355,7 @@
         <v>240</v>
       </c>
       <c r="D75" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
@@ -4386,7 +4387,7 @@
         <v>240</v>
       </c>
       <c r="D76" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
@@ -4450,7 +4451,7 @@
         <v>226</v>
       </c>
       <c r="D78" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>

</xml_diff>

<commit_message>
Update readme, and make the rules *sparkle*
</commit_message>
<xml_diff>
--- a/SCP_ The Downfall of Site 13 Cards.xlsx
+++ b/SCP_ The Downfall of Site 13 Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achyt\dev\Downfall-Of-Site-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53790174-BE5A-4925-93F4-52B89FE53565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E854688-B44D-4FD9-A3DC-09CABF71FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,9 +544,6 @@
     <t>O5-3</t>
   </si>
   <si>
-    <t>O5-3 may be played if there are no "Knowledge" items in play. When put into play, search the item deck for a "Knoweldge" item and put it into play, then shuffle the item deck..</t>
-  </si>
-  <si>
     <t>O5-4</t>
   </si>
   <si>
@@ -625,9 +622,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Choose an item at random. Neutralize the item, but remove it from the game instead of placing it at the bottom of the Item deck</t>
-  </si>
-  <si>
     <t>SCP-682 Breach</t>
   </si>
   <si>
@@ -1273,9 +1267,6 @@
     <t xml:space="preserve">Select an Item in play at random. Neutralize that item. Select a Thaumiel item from the Item deck and put it into play. Shuffle the item deck. </t>
   </si>
   <si>
-    <t>Look at the top of the Item deck. Put that item into play. If that item is a Knowledge item, repeat this card's effect.</t>
-  </si>
-  <si>
     <t>MTF Standing By</t>
   </si>
   <si>
@@ -1292,6 +1283,15 @@
   </si>
   <si>
     <t>icons/sets/set_main.png</t>
+  </si>
+  <si>
+    <t>Choose an item at random. Neutralize the item, but remove it from the game instead of moveing it anywhere else.</t>
+  </si>
+  <si>
+    <t>Add a new Item to containment. If that item is a Knowledge item, repeat this card's effect.</t>
+  </si>
+  <si>
+    <t>O5-3 may be played if there are no "Knowledge" items in play. When put into play, search the item deck for a "Knoweldge" item and put it into play, then shuffle the item deck.</t>
   </si>
 </sst>
 </file>
@@ -1412,46 +1412,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC27BA0"/>
-          <bgColor rgb="FFC27BA0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6B26B"/>
-          <bgColor rgb="FFF6B26B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1503,6 +1463,11 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1520,11 +1485,46 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC27BA0"/>
+          <bgColor rgb="FFC27BA0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6B26B"/>
+          <bgColor rgb="FFF6B26B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1578,14 +1578,14 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Class"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Target"/>
-    <tableColumn id="14" xr3:uid="{B143D954-46E4-4679-BF26-B2E43C92B51E}" name="SpecialLabel" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{B143D954-46E4-4679-BF26-B2E43C92B51E}" name="SpecialLabel" dataDxfId="5"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Rules Text"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Flavor" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Flavor" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Frame"/>
-    <tableColumn id="12" xr3:uid="{3FED4BA4-429D-4286-A8B4-46BA7A594DCA}" name="TopImage" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{3FED4BA4-429D-4286-A8B4-46BA7A594DCA}" name="TopImage" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Art"/>
-    <tableColumn id="16" xr3:uid="{4F636FEA-D81B-4B57-B1AC-DC4A7D4D52B2}" name="CardIcon" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{810D3C9C-9CEF-4430-825E-2B15B40DD1FA}" name="Copy Credits" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{4F636FEA-D81B-4B57-B1AC-DC4A7D4D52B2}" name="CardIcon" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{810D3C9C-9CEF-4430-825E-2B15B40DD1FA}" name="Copy Credits" dataDxfId="1"/>
     <tableColumn id="17" xr3:uid="{BB6A8ECF-0022-4474-BB6E-AE5D22ED4A89}" name="Set Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -1795,9 +1795,9 @@
   </sheetPr>
   <dimension ref="A1:AG864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N92" sqref="N92"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1827,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1836,7 +1836,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
@@ -1848,19 +1848,19 @@
         <v>7</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="O1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
@@ -1880,7 +1880,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="13" t="s">
@@ -1890,19 +1890,19 @@
         <v>14</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
@@ -1940,7 +1940,7 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="13" t="s">
@@ -1950,19 +1950,19 @@
         <v>14</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
@@ -2000,7 +2000,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>23</v>
@@ -2012,19 +2012,19 @@
         <v>14</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -2062,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="13" t="s">
@@ -2072,19 +2072,19 @@
         <v>14</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -2122,7 +2122,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>30</v>
@@ -2134,19 +2134,19 @@
         <v>14</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
@@ -2184,10 +2184,10 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>35</v>
@@ -2196,19 +2196,19 @@
         <v>14</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
@@ -2246,7 +2246,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>38</v>
@@ -2258,19 +2258,19 @@
         <v>14</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
@@ -2308,7 +2308,7 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>41</v>
@@ -2320,19 +2320,19 @@
         <v>14</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
@@ -2370,10 +2370,10 @@
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>45</v>
@@ -2382,19 +2382,19 @@
         <v>14</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
@@ -2432,7 +2432,7 @@
         <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>48</v>
@@ -2444,19 +2444,19 @@
         <v>14</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>51</v>
@@ -2506,19 +2506,19 @@
         <v>14</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
@@ -2556,7 +2556,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>54</v>
@@ -2568,19 +2568,19 @@
         <v>14</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
@@ -2616,7 +2616,7 @@
         <v>57</v>
       </c>
       <c r="G14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>58</v>
@@ -2628,19 +2628,19 @@
         <v>14</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
@@ -2678,7 +2678,7 @@
         <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>61</v>
@@ -2690,19 +2690,19 @@
         <v>14</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
@@ -2740,7 +2740,7 @@
         <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>64</v>
@@ -2752,19 +2752,19 @@
         <v>14</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -2802,7 +2802,7 @@
         <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>67</v>
@@ -2814,19 +2814,19 @@
         <v>14</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -2862,7 +2862,7 @@
         <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>70</v>
@@ -2874,19 +2874,19 @@
         <v>14</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -2921,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>73</v>
@@ -2936,19 +2936,19 @@
         <v>14</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
@@ -2984,31 +2984,31 @@
         <v>57</v>
       </c>
       <c r="G20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
@@ -3046,7 +3046,7 @@
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>77</v>
@@ -3056,19 +3056,19 @@
         <v>14</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="22" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>10</v>
@@ -3104,29 +3104,29 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="23" spans="1:33" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>10</v>
@@ -3159,34 +3159,34 @@
         <v>1</v>
       </c>
       <c r="E23" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G23" t="s">
+        <v>341</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="G23" t="s">
-        <v>343</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>298</v>
-      </c>
       <c r="I23" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="24" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>10</v>
@@ -3224,31 +3224,31 @@
         <v>57</v>
       </c>
       <c r="G24" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="25" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>10</v>
@@ -3284,31 +3284,31 @@
         <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="26" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>10</v>
@@ -3344,31 +3344,31 @@
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="27" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>10</v>
@@ -3404,31 +3404,31 @@
         <v>57</v>
       </c>
       <c r="G27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="28" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>10</v>
@@ -3466,31 +3466,31 @@
         <v>79</v>
       </c>
       <c r="G28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
@@ -3526,7 +3526,7 @@
         <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>80</v>
@@ -3538,19 +3538,19 @@
         <v>14</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -3587,10 +3587,10 @@
         <v>4</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>84</v>
@@ -3599,19 +3599,19 @@
         <v>14</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
         <v>5</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>87</v>
@@ -3644,19 +3644,19 @@
         <v>14</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
@@ -3675,10 +3675,10 @@
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>90</v>
@@ -3687,24 +3687,24 @@
         <v>14</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>83</v>
@@ -3720,7 +3720,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>92</v>
@@ -3732,19 +3732,19 @@
         <v>14</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -3765,7 +3765,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>96</v>
@@ -3777,19 +3777,19 @@
         <v>14</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3810,7 +3810,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>99</v>
@@ -3822,19 +3822,19 @@
         <v>14</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -3855,7 +3855,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>103</v>
@@ -3867,19 +3867,19 @@
         <v>14</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -3898,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>106</v>
@@ -3910,19 +3910,19 @@
         <v>14</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -3941,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="12" t="s">
@@ -3951,19 +3951,19 @@
         <v>14</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -3982,10 +3982,10 @@
         <v>4</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>111</v>
@@ -3994,19 +3994,19 @@
         <v>14</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -4025,36 +4025,36 @@
         <v>5</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>83</v>
@@ -4070,31 +4070,31 @@
         <v>3</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4120,20 +4120,20 @@
         <v>117</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M42" s="6"/>
       <c r="N42" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4159,20 +4159,20 @@
         <v>120</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M43" s="6"/>
       <c r="N43" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4198,20 +4198,20 @@
         <v>123</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M44" s="6"/>
       <c r="N44" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -4231,26 +4231,26 @@
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M45" s="6"/>
       <c r="N45" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
@@ -4276,20 +4276,20 @@
         <v>128</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M46" s="6"/>
       <c r="N46" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4300,7 +4300,7 @@
         <v>114</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D47" s="1">
         <v>4</v>
@@ -4315,20 +4315,20 @@
         <v>131</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M47" s="6"/>
       <c r="N47" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -4346,26 +4346,26 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I48" s="12" t="s">
         <v>133</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M48" s="6"/>
       <c r="N48" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4383,26 +4383,26 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M49" s="6"/>
       <c r="N49" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4413,7 +4413,7 @@
         <v>114</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D50" s="1">
         <v>3</v>
@@ -4428,20 +4428,20 @@
         <v>137</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M50" s="6"/>
       <c r="N50" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4459,26 +4459,26 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I51" s="12" t="s">
         <v>139</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M51" s="6"/>
       <c r="N51" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -4502,25 +4502,25 @@
         <v>142</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M52" s="6"/>
       <c r="N52" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>114</v>
@@ -4533,26 +4533,26 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="I53" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="I53" s="12" t="s">
-        <v>404</v>
-      </c>
       <c r="J53" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M53" s="6"/>
       <c r="N53" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -4575,25 +4575,25 @@
         <v>145</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -4616,25 +4616,25 @@
         <v>147</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K55" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4657,25 +4657,25 @@
         <v>149</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="165.75" x14ac:dyDescent="0.2">
@@ -4695,28 +4695,28 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
@@ -4739,25 +4739,25 @@
         <v>152</v>
       </c>
       <c r="I58" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="M58" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="J58" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="K58" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="L58" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="M58" s="6" t="s">
-        <v>379</v>
-      </c>
       <c r="N58" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O58" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4780,36 +4780,36 @@
         <v>156</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>154</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D60" s="11">
         <v>1</v>
@@ -4818,28 +4818,28 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4859,33 +4859,33 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O61" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>154</v>
@@ -4900,33 +4900,33 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K62" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="L62" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="I62" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="K62" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="L62" s="6" t="s">
-        <v>337</v>
-      </c>
       <c r="M62" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>154</v>
@@ -4941,28 +4941,28 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M63" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4982,28 +4982,28 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
@@ -5026,25 +5026,25 @@
         <v>161</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L65" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M65" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O65" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
@@ -5065,25 +5065,25 @@
         <v>163</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -5106,25 +5106,25 @@
         <v>166</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L67" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M67" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
@@ -5147,25 +5147,25 @@
         <v>168</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M68" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
@@ -5185,33 +5185,33 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="2" t="s">
-        <v>170</v>
+        <v>419</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L69" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M69" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>154</v>
@@ -5226,33 +5226,33 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K70" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O70" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>154</v>
@@ -5267,33 +5267,33 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L71" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O71" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>154</v>
@@ -5308,33 +5308,33 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L72" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M72" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O72" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>154</v>
@@ -5349,33 +5349,33 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I73" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="I73" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="J73" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O73" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>154</v>
@@ -5390,33 +5390,33 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I74" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N74" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O74" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>154</v>
@@ -5431,33 +5431,33 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I75" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="I75" s="12" t="s">
-        <v>184</v>
-      </c>
       <c r="J75" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K75" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M75" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O75" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>154</v>
@@ -5472,33 +5472,33 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I76" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="I76" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="J76" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L76" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M76" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O76" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>154</v>
@@ -5513,33 +5513,33 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
       <c r="H77" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I77" s="19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M77" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O77" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>154</v>
@@ -5554,33 +5554,33 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I78" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="I78" s="12" t="s">
-        <v>192</v>
-      </c>
       <c r="J78" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K78" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L78" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M78" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O78" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>154</v>
@@ -5595,81 +5595,81 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
       <c r="H79" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K79" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="N79" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O79" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I79" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="J79" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="K79" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="L79" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="M79" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="N79" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="O79" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C80" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D80" s="1">
         <v>5</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>197</v>
+        <v>417</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M80" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N80" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O80" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C81" s="9"/>
       <c r="D81" s="1">
@@ -5679,124 +5679,124 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I81" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K81" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M81" s="6"/>
       <c r="N81" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O81" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D82" s="1">
         <v>4</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K82" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L82" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M82" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="N82" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O82" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D83" s="1">
         <v>2</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F83" s="9"/>
       <c r="G83" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I83" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K83" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L83" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O83" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" s="1">
@@ -5806,34 +5806,34 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K84" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L84" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M84" s="6"/>
       <c r="N84" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O84" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C85" s="9"/>
       <c r="D85" s="1">
@@ -5843,206 +5843,206 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K85" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L85" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M85" s="6"/>
       <c r="N85" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O85" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D86" s="1">
         <v>3</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F86" s="9"/>
       <c r="G86" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K86" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O86" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K87" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L87" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M87" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O87" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D88" s="1">
         <v>5</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F88" s="9"/>
       <c r="G88" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J88" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K88" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M88" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O88" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D89" s="1">
         <v>2</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F89" s="9"/>
       <c r="G89" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K89" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L89" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M89" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O89" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
@@ -19222,27 +19222,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B62 C63:C79 B80:B864">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Item"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B62 C63:C79 B80:B864">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Action"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B864">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Character">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Character">
       <formula>NOT(ISERROR(SEARCH(("Character"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B864">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Procedure">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Procedure">
       <formula>NOT(ISERROR(SEARCH(("Procedure"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B864">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Event">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Event">
       <formula>NOT(ISERROR(SEARCH(("Event"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>